<commit_message>
learn how to sum up cells
</commit_message>
<xml_diff>
--- a/Project-1.xlsx
+++ b/Project-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Desktop\Learning Excel\excel-exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB5DD21-AD93-4DB8-8CB7-342E52F46728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F66B5B-FECD-44C4-A5C4-F6D39A5997D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7BDB811D-95D9-48C3-9726-37E9EF4607BC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Monthly Budget</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>August-2022</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -415,20 +418,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D46F3BD-4151-4600-925F-A8361B6312C9}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -444,8 +447,11 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -458,8 +464,16 @@
       <c r="D4">
         <v>325</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4">
+        <f>B4+C4+D4</f>
+        <v>975</v>
+      </c>
+      <c r="F4">
+        <f>E4/$E$8</f>
+        <v>0.20461699895068206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -472,8 +486,16 @@
       <c r="D5">
         <v>175</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5">
+        <f t="shared" ref="E5:E7" si="0">B5+C5+D5</f>
+        <v>500</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F7" si="1">E5/$E$8</f>
+        <v>0.1049317943336831</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -486,8 +508,16 @@
       <c r="D6">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>6.0860440713536204E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -500,10 +530,38 @@
       <c r="D7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.62959076600209862</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
+      </c>
+      <c r="B8">
+        <f>B4+B5+B6+B7</f>
+        <v>1550</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:E8" si="2">C4+C5+C6+C7</f>
+        <v>1635</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>1580</v>
+      </c>
+      <c r="E8">
+        <f>B8+C8+D8</f>
+        <v>4765</v>
+      </c>
+      <c r="F8">
+        <f>E8/$E$8</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
learn new excel functions
</commit_message>
<xml_diff>
--- a/Project-1.xlsx
+++ b/Project-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Desktop\Learning Excel\excel-exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3128CE-76EC-4C9B-B0B2-077A0A43F49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BBA2A3-FCB0-4F71-82EA-48C21808CF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7BDB811D-95D9-48C3-9726-37E9EF4607BC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{7BDB811D-95D9-48C3-9726-37E9EF4607BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Monthly Budget</t>
   </si>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>COUNT</t>
   </si>
 </sst>
 </file>
@@ -418,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D46F3BD-4151-4600-925F-A8361B6312C9}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -564,6 +576,42 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <f>MIN(B4:B7)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <f>MAX(B4:B7)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <f>AVERAGE(B4:B7)</f>
+        <v>387.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <f>COUNT(B4:B7)</f>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>